<commit_message>
cadastro de colab e update criados
</commit_message>
<xml_diff>
--- a/dados/RegistrosColaboradores.xlsx
+++ b/dados/RegistrosColaboradores.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,14 +638,55 @@
           <t>test</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01/01/2023</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>LUIS SANTANA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>